<commit_message>
cap nhat file template mau
</commit_message>
<xml_diff>
--- a/public/download/candidate.xlsx
+++ b/public/download/candidate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinh Nguyen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9D8C07-F50F-44DD-B688-F5F48612CD24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D393008A-309B-48E3-8A90-B5E191E66620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>STT</t>
   </si>
@@ -81,34 +81,34 @@
     <t>Ngày khám sức khoẻ</t>
   </si>
   <si>
-    <t>NGUYỄN THANH</t>
-  </si>
-  <si>
-    <t>TÙNG</t>
-  </si>
-  <si>
-    <t>thanhtung@hcmut.edu.vn</t>
-  </si>
-  <si>
-    <t>0348200824</t>
-  </si>
-  <si>
     <t>Việt Nam</t>
   </si>
   <si>
-    <t>Sài Gòn</t>
-  </si>
-  <si>
-    <t>Nam</t>
-  </si>
-  <si>
     <t>Giới tính(nam hoặc nữ)</t>
   </si>
   <si>
     <t>Có giấy khám sức khoẻ chưa ? (có hoặc chưa)</t>
   </si>
   <si>
-    <t>Có</t>
+    <t>có</t>
+  </si>
+  <si>
+    <t>nam</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>example@gmail.com</t>
+  </si>
+  <si>
+    <t>0912345678</t>
+  </si>
+  <si>
+    <t>TP Hồ Chí Minh</t>
   </si>
 </sst>
 </file>
@@ -184,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -193,6 +193,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -523,8 +524,12 @@
     <col min="6" max="6" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.54296875" customWidth="1"/>
     <col min="8" max="8" width="10.7265625" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="9" max="9" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="36.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -546,7 +551,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -579,7 +584,7 @@
         <v>14</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>15</v>
@@ -590,66 +595,679 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="4">
+        <v>25569</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2">
+        <v>123456789</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="4">
+        <v>43641</v>
+      </c>
+      <c r="N2">
+        <v>123456789</v>
+      </c>
+      <c r="O2" s="4">
+        <v>44007</v>
+      </c>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="4">
-        <v>36336</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="4">
-        <v>36336</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
+      <c r="R2" s="4">
+        <v>44007</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="G3" s="4"/>
       <c r="H3" s="5"/>
       <c r="M3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
       <c r="M4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="M5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="M6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+      <c r="M7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G8" s="4"/>
+      <c r="H8" s="5"/>
+      <c r="M8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G9" s="4"/>
+      <c r="H9" s="5"/>
+      <c r="M9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="M10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G11" s="4"/>
+      <c r="H11" s="5"/>
+      <c r="M11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="R11" s="4"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+      <c r="M12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="R12" s="4"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G13" s="4"/>
+      <c r="H13" s="5"/>
+      <c r="M13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G14" s="4"/>
+      <c r="H14" s="5"/>
+      <c r="M14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G15" s="4"/>
+      <c r="H15" s="5"/>
+      <c r="M15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+      <c r="M16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G17" s="4"/>
+      <c r="H17" s="5"/>
+      <c r="M17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G18" s="4"/>
+      <c r="H18" s="5"/>
+      <c r="M18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G19" s="4"/>
+      <c r="H19" s="5"/>
+      <c r="M19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G20" s="4"/>
+      <c r="H20" s="5"/>
+      <c r="M20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="R20" s="4"/>
+    </row>
+    <row r="21" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G21" s="4"/>
+      <c r="H21" s="5"/>
+      <c r="M21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="R21" s="4"/>
+    </row>
+    <row r="22" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G22" s="4"/>
+      <c r="H22" s="5"/>
+      <c r="M22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="R22" s="4"/>
+    </row>
+    <row r="23" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G23" s="4"/>
+      <c r="H23" s="5"/>
+      <c r="M23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="R23" s="4"/>
+    </row>
+    <row r="24" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G24" s="4"/>
+      <c r="H24" s="5"/>
+      <c r="M24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="R24" s="4"/>
+    </row>
+    <row r="25" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G25" s="4"/>
+      <c r="H25" s="5"/>
+      <c r="M25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="R25" s="4"/>
+    </row>
+    <row r="26" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
+      <c r="M26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="R26" s="4"/>
+    </row>
+    <row r="27" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G27" s="4"/>
+      <c r="H27" s="5"/>
+      <c r="M27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="R27" s="4"/>
+    </row>
+    <row r="28" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G28" s="4"/>
+      <c r="H28" s="5"/>
+      <c r="M28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="R28" s="4"/>
+    </row>
+    <row r="29" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G29" s="4"/>
+      <c r="H29" s="5"/>
+      <c r="M29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="R29" s="4"/>
+    </row>
+    <row r="30" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G30" s="4"/>
+      <c r="H30" s="5"/>
+      <c r="M30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="R30" s="4"/>
+    </row>
+    <row r="31" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G31" s="4"/>
+      <c r="H31" s="5"/>
+      <c r="M31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="R31" s="4"/>
+    </row>
+    <row r="32" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G32" s="4"/>
+      <c r="H32" s="5"/>
+      <c r="M32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="R32" s="4"/>
+    </row>
+    <row r="33" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G33" s="4"/>
+      <c r="H33" s="5"/>
+      <c r="M33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="R33" s="4"/>
+    </row>
+    <row r="34" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G34" s="4"/>
+      <c r="H34" s="5"/>
+      <c r="M34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="R34" s="4"/>
+    </row>
+    <row r="35" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G35" s="4"/>
+      <c r="H35" s="5"/>
+      <c r="M35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="R35" s="4"/>
+    </row>
+    <row r="36" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G36" s="4"/>
+      <c r="H36" s="5"/>
+      <c r="M36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="R36" s="4"/>
+    </row>
+    <row r="37" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G37" s="4"/>
+      <c r="H37" s="5"/>
+      <c r="M37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="R37" s="4"/>
+    </row>
+    <row r="38" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G38" s="4"/>
+      <c r="H38" s="5"/>
+      <c r="M38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="R38" s="4"/>
+    </row>
+    <row r="39" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G39" s="4"/>
+      <c r="H39" s="5"/>
+      <c r="M39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="R39" s="4"/>
+    </row>
+    <row r="40" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G40" s="4"/>
+      <c r="H40" s="5"/>
+      <c r="M40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="R40" s="4"/>
+    </row>
+    <row r="41" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G41" s="4"/>
+      <c r="H41" s="5"/>
+      <c r="M41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="R41" s="4"/>
+    </row>
+    <row r="42" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G42" s="4"/>
+      <c r="H42" s="5"/>
+      <c r="M42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="R42" s="4"/>
+    </row>
+    <row r="43" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G43" s="4"/>
+      <c r="H43" s="5"/>
+      <c r="M43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="R43" s="4"/>
+    </row>
+    <row r="44" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G44" s="4"/>
+      <c r="H44" s="5"/>
+      <c r="M44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="R44" s="4"/>
+    </row>
+    <row r="45" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G45" s="4"/>
+      <c r="H45" s="5"/>
+      <c r="M45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="R45" s="4"/>
+    </row>
+    <row r="46" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G46" s="4"/>
+      <c r="H46" s="5"/>
+      <c r="M46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="R46" s="4"/>
+    </row>
+    <row r="47" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G47" s="4"/>
+      <c r="H47" s="5"/>
+      <c r="M47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="R47" s="4"/>
+    </row>
+    <row r="48" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G48" s="4"/>
+      <c r="H48" s="5"/>
+      <c r="M48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="R48" s="4"/>
+    </row>
+    <row r="49" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G49" s="4"/>
+      <c r="H49" s="5"/>
+      <c r="M49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="R49" s="4"/>
+    </row>
+    <row r="50" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G50" s="4"/>
+      <c r="H50" s="5"/>
+      <c r="M50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="R50" s="4"/>
+    </row>
+    <row r="51" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G51" s="4"/>
+      <c r="H51" s="5"/>
+      <c r="M51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="R51" s="4"/>
+    </row>
+    <row r="52" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G52" s="4"/>
+      <c r="H52" s="5"/>
+      <c r="M52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="R52" s="4"/>
+    </row>
+    <row r="53" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G53" s="4"/>
+      <c r="H53" s="5"/>
+      <c r="M53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="R53" s="4"/>
+    </row>
+    <row r="54" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G54" s="4"/>
+      <c r="H54" s="5"/>
+      <c r="M54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="R54" s="4"/>
+    </row>
+    <row r="55" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G55" s="4"/>
+      <c r="H55" s="5"/>
+      <c r="M55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="R55" s="4"/>
+    </row>
+    <row r="56" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G56" s="4"/>
+      <c r="H56" s="5"/>
+      <c r="M56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="R56" s="4"/>
+    </row>
+    <row r="57" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G57" s="4"/>
+      <c r="H57" s="5"/>
+      <c r="M57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="R57" s="4"/>
+    </row>
+    <row r="58" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G58" s="4"/>
+      <c r="H58" s="5"/>
+      <c r="M58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="R58" s="4"/>
+    </row>
+    <row r="59" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G59" s="4"/>
+      <c r="H59" s="5"/>
+      <c r="M59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="R59" s="4"/>
+    </row>
+    <row r="60" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G60" s="4"/>
+      <c r="H60" s="5"/>
+      <c r="M60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="R60" s="4"/>
+    </row>
+    <row r="61" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G61" s="4"/>
+      <c r="H61" s="5"/>
+      <c r="M61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="R61" s="4"/>
+    </row>
+    <row r="62" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G62" s="4"/>
+      <c r="H62" s="5"/>
+      <c r="M62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="R62" s="4"/>
+    </row>
+    <row r="63" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G63" s="4"/>
+      <c r="H63" s="5"/>
+      <c r="M63" s="4"/>
+      <c r="O63" s="4"/>
+      <c r="R63" s="4"/>
+    </row>
+    <row r="64" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G64" s="4"/>
+      <c r="H64" s="5"/>
+      <c r="M64" s="4"/>
+      <c r="O64" s="4"/>
+      <c r="R64" s="4"/>
+    </row>
+    <row r="65" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G65" s="4"/>
+      <c r="H65" s="5"/>
+      <c r="M65" s="4"/>
+      <c r="O65" s="4"/>
+      <c r="R65" s="4"/>
+    </row>
+    <row r="66" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G66" s="4"/>
+      <c r="H66" s="5"/>
+      <c r="M66" s="4"/>
+      <c r="O66" s="4"/>
+      <c r="R66" s="4"/>
+    </row>
+    <row r="67" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G67" s="4"/>
+      <c r="H67" s="5"/>
+      <c r="M67" s="4"/>
+      <c r="O67" s="4"/>
+      <c r="R67" s="4"/>
+    </row>
+    <row r="68" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G68" s="4"/>
+      <c r="H68" s="5"/>
+      <c r="M68" s="4"/>
+      <c r="O68" s="4"/>
+      <c r="R68" s="4"/>
+    </row>
+    <row r="69" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G69" s="4"/>
+      <c r="H69" s="5"/>
+      <c r="M69" s="4"/>
+      <c r="O69" s="4"/>
+      <c r="R69" s="4"/>
+    </row>
+    <row r="70" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G70" s="4"/>
+      <c r="H70" s="5"/>
+      <c r="M70" s="4"/>
+      <c r="O70" s="4"/>
+      <c r="R70" s="4"/>
+    </row>
+    <row r="71" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G71" s="4"/>
+      <c r="H71" s="5"/>
+      <c r="M71" s="4"/>
+      <c r="O71" s="4"/>
+      <c r="R71" s="4"/>
+    </row>
+    <row r="72" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G72" s="4"/>
+      <c r="H72" s="5"/>
+      <c r="M72" s="4"/>
+      <c r="O72" s="4"/>
+      <c r="R72" s="4"/>
+    </row>
+    <row r="73" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G73" s="4"/>
+      <c r="H73" s="5"/>
+      <c r="M73" s="4"/>
+      <c r="O73" s="4"/>
+      <c r="R73" s="4"/>
+    </row>
+    <row r="74" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G74" s="4"/>
+      <c r="H74" s="5"/>
+      <c r="M74" s="4"/>
+      <c r="O74" s="4"/>
+      <c r="R74" s="4"/>
+    </row>
+    <row r="75" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G75" s="4"/>
+      <c r="H75" s="5"/>
+      <c r="M75" s="4"/>
+      <c r="O75" s="4"/>
+      <c r="R75" s="4"/>
+    </row>
+    <row r="76" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G76" s="4"/>
+      <c r="H76" s="5"/>
+      <c r="M76" s="4"/>
+      <c r="O76" s="4"/>
+      <c r="R76" s="4"/>
+    </row>
+    <row r="77" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G77" s="4"/>
+      <c r="H77" s="5"/>
+      <c r="M77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="R77" s="4"/>
+    </row>
+    <row r="78" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G78" s="4"/>
+      <c r="H78" s="5"/>
+      <c r="M78" s="4"/>
+      <c r="O78" s="4"/>
+      <c r="R78" s="4"/>
+    </row>
+    <row r="79" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G79" s="4"/>
+      <c r="H79" s="5"/>
+      <c r="M79" s="4"/>
+      <c r="O79" s="4"/>
+      <c r="R79" s="4"/>
+    </row>
+    <row r="80" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G80" s="4"/>
+      <c r="H80" s="5"/>
+      <c r="M80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="R80" s="4"/>
+    </row>
+    <row r="81" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G81" s="4"/>
+      <c r="H81" s="5"/>
+      <c r="M81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="R81" s="4"/>
+    </row>
+    <row r="82" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G82" s="4"/>
+      <c r="H82" s="5"/>
+      <c r="M82" s="4"/>
+      <c r="O82" s="4"/>
+      <c r="R82" s="4"/>
+    </row>
+    <row r="83" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G83" s="4"/>
+      <c r="H83" s="5"/>
+      <c r="M83" s="4"/>
+      <c r="O83" s="4"/>
+      <c r="R83" s="4"/>
+    </row>
+    <row r="84" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G84" s="4"/>
+      <c r="H84" s="5"/>
+      <c r="M84" s="4"/>
+      <c r="O84" s="4"/>
+      <c r="R84" s="4"/>
+    </row>
+    <row r="85" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G85" s="4"/>
+      <c r="H85" s="5"/>
+      <c r="M85" s="4"/>
+      <c r="O85" s="4"/>
+      <c r="R85" s="4"/>
+    </row>
+    <row r="86" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G86" s="4"/>
+      <c r="H86" s="5"/>
+      <c r="M86" s="4"/>
+      <c r="O86" s="4"/>
+      <c r="R86" s="4"/>
+    </row>
+    <row r="87" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G87" s="4"/>
+      <c r="H87" s="5"/>
+      <c r="M87" s="4"/>
+      <c r="O87" s="4"/>
+      <c r="R87" s="4"/>
+    </row>
+    <row r="88" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G88" s="4"/>
+      <c r="H88" s="5"/>
+      <c r="M88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="R88" s="4"/>
+    </row>
+    <row r="89" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G89" s="4"/>
+      <c r="H89" s="5"/>
+      <c r="M89" s="4"/>
+      <c r="O89" s="4"/>
+      <c r="R89" s="4"/>
+    </row>
+    <row r="90" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G90" s="4"/>
+      <c r="H90" s="5"/>
+      <c r="M90" s="4"/>
+      <c r="O90" s="4"/>
+      <c r="R90" s="4"/>
+    </row>
+    <row r="91" spans="7:18" x14ac:dyDescent="0.35">
+      <c r="G91" s="4"/>
+      <c r="H91" s="5"/>
+      <c r="M91" s="4"/>
+      <c r="O91" s="4"/>
+      <c r="R91" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
lam lai form dang nhap
</commit_message>
<xml_diff>
--- a/public/download/candidate.xlsx
+++ b/public/download/candidate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinh Nguyen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856055BE-08DA-418A-B5B5-F60244923764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4B99A5-B805-4AFF-823F-C3C8B06231F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>STT</t>
   </si>
@@ -48,19 +48,16 @@
     <t>Nơi đăng ký hộ khẩu thường trú</t>
   </si>
   <si>
-    <t>Số CMND, CCCD</t>
-  </si>
-  <si>
     <t>Nơi cấp CMND, CCCD</t>
   </si>
   <si>
-    <t>Số giấy phép lái xe 2 bánh</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Nơi cấp giấy phép lái xe 2 bánh</t>
   </si>
   <si>
     <t>Việt Nam</t>
+  </si>
+  <si>
+    <t>nam</t>
   </si>
   <si>
     <t>Nguyễn Văn</t>
@@ -125,10 +122,13 @@
 ('dd/mm/yyyy)</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>NAM</t>
+    <t>Số CMND, CCCD('xxx)</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>Số giấy phép lái xe 2 bánh('xxx)</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="A1:T91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -584,13 +584,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>4</v>
@@ -602,34 +602,34 @@
         <v>6</v>
       </c>
       <c r="K1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>10</v>
-      </c>
       <c r="Q1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
@@ -637,58 +637,58 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2">
-        <v>123456789</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N2">
-        <v>123456789</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="P2" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S2" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
lịch nghỉ của giáo viên và lịch học của học viên
</commit_message>
<xml_diff>
--- a/public/download/candidate.xlsx
+++ b/public/download/candidate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>STT</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Tên của cố vấn học tập dự kiến</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Học phí phải đóng </t>
   </si>
   <si>
     <t>Nguyễn Văn</t>
@@ -139,8 +142,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="dd/mm/yy"/>
   </numFmts>
@@ -173,10 +176,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -189,6 +192,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,10 +222,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -257,6 +268,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -266,51 +313,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,61 +334,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,115 +508,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,15 +537,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -554,6 +548,26 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -597,17 +611,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -634,15 +637,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -652,130 +655,130 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1115,10 +1118,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V91"/>
+  <dimension ref="A1:W91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="V2" sqref="U1:V2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5047619047619" defaultRowHeight="15"/>
@@ -1144,9 +1147,10 @@
     <col min="20" max="20" width="20" customWidth="1"/>
     <col min="21" max="21" width="22" customWidth="1"/>
     <col min="22" max="22" width="13.7142857142857" customWidth="1"/>
+    <col min="23" max="23" width="14.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="38.25" spans="1:22">
+    <row r="1" s="1" customFormat="1" ht="38.25" spans="1:23">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1213,67 +1217,73 @@
       <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
       <c r="M2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" t="s">
-        <v>29</v>
-      </c>
       <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="S2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="W2">
+        <v>14000000</v>
       </c>
     </row>
     <row r="3" spans="8:18">

</xml_diff>